<commit_message>
Adds RPT_TXIO_DDAC_TAB query and related files
Adds a new SQL query to extract data from RPT_TXIO_DDAC_TAB
and related sumap data, focusing on specific conditions
such as SIGUMGO_ORG_C, ICH_SIGUMGO_GUN_GU_C, SGG_ACNO and
date ranges.

Includes creation of new Excel files related to sunap data
and updates existing Excel file.
</commit_message>
<xml_diff>
--- a/춘천시상수도1031수납집계데이터20251125.xlsx
+++ b/춘천시상수도1031수납집계데이터20251125.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA6A3254-DED6-47F8-A0C4-F33957F9D0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839BF6D0-BE80-4EAD-8ACC-E2AFC2EA956D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>SUNAP_DT</t>
   </si>
@@ -31,620 +44,461 @@
     <t>20250102</t>
   </si>
   <si>
-    <t>169977990</t>
-  </si>
-  <si>
     <t>20250103</t>
   </si>
   <si>
-    <t>4244000</t>
-  </si>
-  <si>
     <t>20250109</t>
   </si>
   <si>
-    <t>93162630</t>
-  </si>
-  <si>
     <t>20250113</t>
   </si>
   <si>
-    <t>1838350</t>
-  </si>
-  <si>
     <t>20250114</t>
   </si>
   <si>
-    <t>9152120</t>
-  </si>
-  <si>
     <t>20250115</t>
   </si>
   <si>
-    <t>10549320</t>
-  </si>
-  <si>
     <t>20250116</t>
   </si>
   <si>
-    <t>19383110</t>
-  </si>
-  <si>
     <t>20250117</t>
   </si>
   <si>
-    <t>30276490</t>
-  </si>
-  <si>
     <t>20250120</t>
   </si>
   <si>
-    <t>46424530</t>
-  </si>
-  <si>
     <t>20250121</t>
   </si>
   <si>
-    <t>40945860</t>
-  </si>
-  <si>
     <t>20250122</t>
   </si>
   <si>
-    <t>129573410</t>
-  </si>
-  <si>
     <t>20250123</t>
   </si>
   <si>
-    <t>45593690</t>
-  </si>
-  <si>
     <t>20250124</t>
   </si>
   <si>
-    <t>140431130</t>
-  </si>
-  <si>
     <t>20250131</t>
   </si>
   <si>
-    <t>1772805680</t>
-  </si>
-  <si>
     <t>20250210</t>
   </si>
   <si>
-    <t>52777850</t>
-  </si>
-  <si>
     <t>20250212</t>
   </si>
   <si>
-    <t>8451150</t>
-  </si>
-  <si>
     <t>20250213</t>
   </si>
   <si>
-    <t>9583850</t>
-  </si>
-  <si>
     <t>20250214</t>
   </si>
   <si>
-    <t>9537650</t>
-  </si>
-  <si>
     <t>20250217</t>
   </si>
   <si>
-    <t>16732480</t>
-  </si>
-  <si>
     <t>20250218</t>
   </si>
   <si>
-    <t>30880350</t>
-  </si>
-  <si>
     <t>20250219</t>
   </si>
   <si>
-    <t>74648560</t>
-  </si>
-  <si>
     <t>20250220</t>
   </si>
   <si>
-    <t>289249500</t>
-  </si>
-  <si>
     <t>20250221</t>
   </si>
   <si>
-    <t>108937290</t>
-  </si>
-  <si>
     <t>20250224</t>
   </si>
   <si>
-    <t>108230980</t>
-  </si>
-  <si>
     <t>20250225</t>
   </si>
   <si>
-    <t>130311570</t>
-  </si>
-  <si>
     <t>20250226</t>
   </si>
   <si>
-    <t>63504870</t>
-  </si>
-  <si>
     <t>20250227</t>
   </si>
   <si>
-    <t>396757640</t>
-  </si>
-  <si>
     <t>20250228</t>
   </si>
   <si>
-    <t>1530507890</t>
-  </si>
-  <si>
     <t>20250310</t>
   </si>
   <si>
-    <t>4706000000</t>
-  </si>
-  <si>
     <t>20250311</t>
   </si>
   <si>
-    <t>64770900</t>
-  </si>
-  <si>
     <t>20250313</t>
   </si>
   <si>
-    <t>19575725</t>
-  </si>
-  <si>
     <t>20250314</t>
   </si>
   <si>
-    <t>29537110</t>
-  </si>
-  <si>
     <t>20250317</t>
   </si>
   <si>
-    <t>38261007</t>
-  </si>
-  <si>
     <t>20250318</t>
   </si>
   <si>
-    <t>295654048</t>
-  </si>
-  <si>
     <t>20250319</t>
   </si>
   <si>
-    <t>115093924</t>
-  </si>
-  <si>
     <t>20250320</t>
   </si>
   <si>
-    <t>38297022</t>
-  </si>
-  <si>
     <t>20250321</t>
   </si>
   <si>
-    <t>35811580</t>
-  </si>
-  <si>
     <t>20250324</t>
   </si>
   <si>
-    <t>105774709</t>
-  </si>
-  <si>
     <t>20250325</t>
   </si>
   <si>
-    <t>49971160</t>
-  </si>
-  <si>
     <t>20250326</t>
   </si>
   <si>
-    <t>8308429220</t>
-  </si>
-  <si>
     <t>20250327</t>
   </si>
   <si>
-    <t>10899088541</t>
-  </si>
-  <si>
     <t>20250328</t>
   </si>
   <si>
-    <t>48202150</t>
-  </si>
-  <si>
     <t>20250331</t>
   </si>
   <si>
-    <t>1732562240</t>
-  </si>
-  <si>
     <t>20250408</t>
   </si>
   <si>
-    <t>86174050</t>
-  </si>
-  <si>
     <t>20250410</t>
   </si>
   <si>
-    <t>49790412</t>
-  </si>
-  <si>
     <t>20250411</t>
   </si>
   <si>
-    <t>4075267430</t>
-  </si>
-  <si>
     <t>20250414</t>
   </si>
   <si>
-    <t>102957970</t>
-  </si>
-  <si>
     <t>20250415</t>
   </si>
   <si>
-    <t>28111470</t>
-  </si>
-  <si>
     <t>20250416</t>
   </si>
   <si>
-    <t>35024700</t>
-  </si>
-  <si>
     <t>20250417</t>
   </si>
   <si>
-    <t>58263360</t>
-  </si>
-  <si>
     <t>20250418</t>
   </si>
   <si>
-    <t>105371640</t>
-  </si>
-  <si>
     <t>20250421</t>
   </si>
   <si>
-    <t>29908580</t>
-  </si>
-  <si>
     <t>20250422</t>
   </si>
   <si>
-    <t>60303980</t>
-  </si>
-  <si>
     <t>20250423</t>
   </si>
   <si>
-    <t>121230680</t>
-  </si>
-  <si>
     <t>20250424</t>
   </si>
   <si>
-    <t>39301670</t>
-  </si>
-  <si>
     <t>20250425</t>
   </si>
   <si>
-    <t>47138910</t>
-  </si>
-  <si>
     <t>20250428</t>
   </si>
   <si>
-    <t>51763450</t>
-  </si>
-  <si>
     <t>20250429</t>
   </si>
   <si>
-    <t>138495980</t>
-  </si>
-  <si>
     <t>20250430</t>
   </si>
   <si>
-    <t>1533263810</t>
-  </si>
-  <si>
     <t>20250513</t>
   </si>
   <si>
-    <t>86075740</t>
-  </si>
-  <si>
     <t>20250514</t>
   </si>
   <si>
-    <t>1650750</t>
-  </si>
-  <si>
     <t>20250515</t>
   </si>
   <si>
-    <t>17885940</t>
-  </si>
-  <si>
     <t>20250516</t>
   </si>
   <si>
-    <t>18070430</t>
-  </si>
-  <si>
     <t>20250519</t>
   </si>
   <si>
-    <t>33786840</t>
-  </si>
-  <si>
     <t>20250520</t>
   </si>
   <si>
-    <t>107298470</t>
-  </si>
-  <si>
     <t>20250521</t>
   </si>
   <si>
-    <t>63059160</t>
-  </si>
-  <si>
     <t>20250522</t>
   </si>
   <si>
-    <t>97169760</t>
-  </si>
-  <si>
     <t>20250523</t>
   </si>
   <si>
-    <t>68661160</t>
-  </si>
-  <si>
     <t>20250526</t>
   </si>
   <si>
-    <t>61565400</t>
-  </si>
-  <si>
     <t>20250527</t>
   </si>
   <si>
-    <t>174059380</t>
-  </si>
-  <si>
     <t>20250528</t>
   </si>
   <si>
-    <t>80426760</t>
-  </si>
-  <si>
     <t>20250529</t>
   </si>
   <si>
-    <t>54327010</t>
-  </si>
-  <si>
     <t>20250530</t>
   </si>
   <si>
-    <t>120279080</t>
-  </si>
-  <si>
     <t>20250531</t>
   </si>
   <si>
-    <t>453681290</t>
-  </si>
-  <si>
     <t>20250602</t>
   </si>
   <si>
-    <t>4570</t>
-  </si>
-  <si>
     <t>20250612</t>
   </si>
   <si>
-    <t>1389294720</t>
-  </si>
-  <si>
     <t>20250616</t>
   </si>
   <si>
-    <t>9269446</t>
-  </si>
-  <si>
     <t>20250617</t>
   </si>
   <si>
-    <t>45065840</t>
-  </si>
-  <si>
     <t>20250618</t>
   </si>
   <si>
-    <t>55320070</t>
-  </si>
-  <si>
     <t>20250619</t>
   </si>
   <si>
-    <t>102898140</t>
-  </si>
-  <si>
     <t>20250620</t>
   </si>
   <si>
-    <t>53996760</t>
-  </si>
-  <si>
     <t>20250623</t>
   </si>
   <si>
-    <t>81306230</t>
-  </si>
-  <si>
     <t>20250624</t>
   </si>
   <si>
-    <t>108531100</t>
-  </si>
-  <si>
     <t>20250625</t>
   </si>
   <si>
-    <t>90544940</t>
-  </si>
-  <si>
     <t>20250626</t>
   </si>
   <si>
-    <t>3485703219</t>
-  </si>
-  <si>
     <t>20250627</t>
   </si>
   <si>
-    <t>211653674</t>
-  </si>
-  <si>
     <t>20250630</t>
   </si>
   <si>
-    <t>1749286000</t>
-  </si>
-  <si>
     <t>20250701</t>
   </si>
   <si>
-    <t>153880350</t>
-  </si>
-  <si>
     <t>20250704</t>
   </si>
   <si>
-    <t>72094</t>
-  </si>
-  <si>
     <t>20250708</t>
   </si>
   <si>
-    <t>134341180</t>
-  </si>
-  <si>
     <t>20250710</t>
   </si>
   <si>
-    <t>12546950</t>
-  </si>
-  <si>
     <t>20250711</t>
   </si>
   <si>
-    <t>38435830</t>
-  </si>
-  <si>
     <t>20250714</t>
   </si>
   <si>
-    <t>12687770</t>
-  </si>
-  <si>
     <t>20250715</t>
   </si>
   <si>
-    <t>23362760</t>
-  </si>
-  <si>
     <t>20250716</t>
   </si>
   <si>
-    <t>53055070</t>
-  </si>
-  <si>
     <t>20250717</t>
   </si>
   <si>
-    <t>35274120</t>
-  </si>
-  <si>
     <t>20250718</t>
   </si>
   <si>
-    <t>80977351</t>
-  </si>
-  <si>
     <t>20250721</t>
   </si>
   <si>
-    <t>46747980</t>
-  </si>
-  <si>
     <t>20250722</t>
   </si>
   <si>
-    <t>36254168</t>
-  </si>
-  <si>
     <t>20250723</t>
   </si>
   <si>
-    <t>138359260</t>
+    <t>20250724</t>
+  </si>
+  <si>
+    <t>20250725</t>
+  </si>
+  <si>
+    <t>20250728</t>
+  </si>
+  <si>
+    <t>20250729</t>
+  </si>
+  <si>
+    <t>20250730</t>
+  </si>
+  <si>
+    <t>20250731</t>
+  </si>
+  <si>
+    <t>20250808</t>
+  </si>
+  <si>
+    <t>20250812</t>
+  </si>
+  <si>
+    <t>20250813</t>
+  </si>
+  <si>
+    <t>20250814</t>
+  </si>
+  <si>
+    <t>20250818</t>
+  </si>
+  <si>
+    <t>20250819</t>
+  </si>
+  <si>
+    <t>20250820</t>
+  </si>
+  <si>
+    <t>20250821</t>
+  </si>
+  <si>
+    <t>20250825</t>
+  </si>
+  <si>
+    <t>20250826</t>
+  </si>
+  <si>
+    <t>20250827</t>
+  </si>
+  <si>
+    <t>20250828</t>
+  </si>
+  <si>
+    <t>20250829</t>
+  </si>
+  <si>
+    <t>20250831</t>
+  </si>
+  <si>
+    <t>20250909</t>
+  </si>
+  <si>
+    <t>20250911</t>
+  </si>
+  <si>
+    <t>20250912</t>
+  </si>
+  <si>
+    <t>20250915</t>
+  </si>
+  <si>
+    <t>20250916</t>
+  </si>
+  <si>
+    <t>20250917</t>
+  </si>
+  <si>
+    <t>20250918</t>
+  </si>
+  <si>
+    <t>20250922</t>
+  </si>
+  <si>
+    <t>20250923</t>
+  </si>
+  <si>
+    <t>20250924</t>
+  </si>
+  <si>
+    <t>20250925</t>
+  </si>
+  <si>
+    <t>20250926</t>
+  </si>
+  <si>
+    <t>20250930</t>
+  </si>
+  <si>
+    <t>20251015</t>
+  </si>
+  <si>
+    <t>20251017</t>
+  </si>
+  <si>
+    <t>20251020</t>
+  </si>
+  <si>
+    <t>20251021</t>
+  </si>
+  <si>
+    <t>20251022</t>
+  </si>
+  <si>
+    <t>20251023</t>
+  </si>
+  <si>
+    <t>20250822</t>
+  </si>
+  <si>
+    <t>20250919</t>
+  </si>
+  <si>
+    <t>20250929</t>
+  </si>
+  <si>
+    <t>20251024</t>
+  </si>
+  <si>
+    <t>20251027</t>
+  </si>
+  <si>
+    <t>20251028</t>
+  </si>
+  <si>
+    <t>20251029</t>
+  </si>
+  <si>
+    <t>20251030</t>
+  </si>
+  <si>
+    <t>20251031</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="179" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
@@ -707,14 +561,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1051,14 +908,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B149" sqref="A1:B149"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1073,804 +932,1188 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="B2" s="3">
+        <v>169977990</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4244000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>93162630</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1838350</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9152120</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10549320</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>19383110</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>30276490</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>46424530</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>40945860</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>129573410</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45593690</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>140431130</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1772805680</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>52777850</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="3">
+        <v>8451150</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="3">
+        <v>9583850</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="3">
+        <v>9537650</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="B20" s="3">
+        <v>16732480</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="3">
+        <v>30880350</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="3">
+        <v>74648560</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="3">
+        <v>289249500</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
+      </c>
+      <c r="B24" s="3">
+        <v>108937290</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
+      </c>
+      <c r="B25" s="3">
+        <v>108230980</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="3">
+        <v>130311570</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="B27" s="3">
+        <v>63504870</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
+      </c>
+      <c r="B28" s="3">
+        <v>396757640</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1530507890</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
+      </c>
+      <c r="B30" s="3">
+        <v>4706000000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>61</v>
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>64770900</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="B32" s="3">
+        <v>19575725</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>33</v>
+      </c>
+      <c r="B33" s="3">
+        <v>29537110</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
+      </c>
+      <c r="B34" s="3">
+        <v>38261007</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="B35" s="3">
+        <v>295654048</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>36</v>
+      </c>
+      <c r="B36" s="3">
+        <v>115093924</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="B37" s="3">
+        <v>38297022</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="3">
+        <v>35811580</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="B39" s="3">
+        <v>105774709</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="3">
+        <v>49971160</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>81</v>
+        <v>41</v>
+      </c>
+      <c r="B41" s="3">
+        <v>8308429220</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>42</v>
+      </c>
+      <c r="B42" s="3">
+        <v>10899088541</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>43</v>
+      </c>
+      <c r="B43" s="3">
+        <v>48202150</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>87</v>
+        <v>44</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1732562240</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>45</v>
+      </c>
+      <c r="B45" s="3">
+        <v>86174050</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
+      </c>
+      <c r="B46" s="3">
+        <v>49790412</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>47</v>
+      </c>
+      <c r="B47" s="3">
+        <v>4075267430</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>48</v>
+      </c>
+      <c r="B48" s="3">
+        <v>102957970</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>49</v>
+      </c>
+      <c r="B49" s="3">
+        <v>28111470</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>50</v>
+      </c>
+      <c r="B50" s="3">
+        <v>35024700</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>51</v>
+      </c>
+      <c r="B51" s="3">
+        <v>58263360</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>52</v>
+      </c>
+      <c r="B52" s="3">
+        <v>105371640</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>53</v>
+      </c>
+      <c r="B53" s="3">
+        <v>29908580</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="B54" s="3">
+        <v>60303980</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>55</v>
+      </c>
+      <c r="B55" s="3">
+        <v>121230680</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>56</v>
+      </c>
+      <c r="B56" s="3">
+        <v>39301670</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>57</v>
+      </c>
+      <c r="B57" s="3">
+        <v>47138910</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B58" s="3">
+        <v>51763450</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>117</v>
+        <v>59</v>
+      </c>
+      <c r="B59" s="3">
+        <v>138495980</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>60</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1533263810</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>61</v>
+      </c>
+      <c r="B61" s="3">
+        <v>86075740</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>123</v>
+        <v>62</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1650750</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>63</v>
+      </c>
+      <c r="B63" s="3">
+        <v>17885940</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>127</v>
+        <v>64</v>
+      </c>
+      <c r="B64" s="3">
+        <v>18070430</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>65</v>
+      </c>
+      <c r="B65" s="3">
+        <v>33786840</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>66</v>
+      </c>
+      <c r="B66" s="3">
+        <v>107298470</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>133</v>
+        <v>67</v>
+      </c>
+      <c r="B67" s="3">
+        <v>63059160</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>135</v>
+        <v>68</v>
+      </c>
+      <c r="B68" s="3">
+        <v>97169760</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>137</v>
+        <v>69</v>
+      </c>
+      <c r="B69" s="3">
+        <v>68661160</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
+      </c>
+      <c r="B70" s="3">
+        <v>61565400</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>141</v>
+        <v>71</v>
+      </c>
+      <c r="B71" s="3">
+        <v>174059380</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>143</v>
+        <v>72</v>
+      </c>
+      <c r="B72" s="3">
+        <v>80426760</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>145</v>
+        <v>73</v>
+      </c>
+      <c r="B73" s="3">
+        <v>54327010</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>147</v>
+        <v>74</v>
+      </c>
+      <c r="B74" s="3">
+        <v>120279080</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>149</v>
+        <v>75</v>
+      </c>
+      <c r="B75" s="3">
+        <v>453681290</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>151</v>
+        <v>76</v>
+      </c>
+      <c r="B76" s="3">
+        <v>4570</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>153</v>
+        <v>77</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1389294720</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>155</v>
+        <v>78</v>
+      </c>
+      <c r="B78" s="3">
+        <v>9269446</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>157</v>
+        <v>79</v>
+      </c>
+      <c r="B79" s="3">
+        <v>45065840</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>159</v>
+        <v>80</v>
+      </c>
+      <c r="B80" s="3">
+        <v>55320070</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>161</v>
+        <v>81</v>
+      </c>
+      <c r="B81" s="3">
+        <v>102898140</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>163</v>
+        <v>82</v>
+      </c>
+      <c r="B82" s="3">
+        <v>53996760</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>165</v>
+        <v>83</v>
+      </c>
+      <c r="B83" s="3">
+        <v>81306230</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>167</v>
+        <v>85</v>
+      </c>
+      <c r="B84" s="3">
+        <v>90544940</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>169</v>
+        <v>86</v>
+      </c>
+      <c r="B85" s="3">
+        <v>3485703219</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>171</v>
+        <v>87</v>
+      </c>
+      <c r="B86" s="3">
+        <v>211653674</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>173</v>
+        <v>88</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1749286000</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>175</v>
+        <v>89</v>
+      </c>
+      <c r="B88" s="3">
+        <v>153880350</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>177</v>
+        <v>90</v>
+      </c>
+      <c r="B89" s="3">
+        <v>72094</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>179</v>
+        <v>91</v>
+      </c>
+      <c r="B90" s="3">
+        <v>134341180</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>181</v>
+        <v>92</v>
+      </c>
+      <c r="B91" s="3">
+        <v>12546950</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>183</v>
+        <v>93</v>
+      </c>
+      <c r="B92" s="3">
+        <v>38435830</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>185</v>
+        <v>94</v>
+      </c>
+      <c r="B93" s="3">
+        <v>12687770</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>187</v>
+        <v>95</v>
+      </c>
+      <c r="B94" s="3">
+        <v>23362760</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>189</v>
+        <v>96</v>
+      </c>
+      <c r="B95" s="3">
+        <v>53055070</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>191</v>
+        <v>97</v>
+      </c>
+      <c r="B96" s="3">
+        <v>35274120</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>193</v>
+        <v>98</v>
+      </c>
+      <c r="B97" s="3">
+        <v>80977351</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>195</v>
+        <v>99</v>
+      </c>
+      <c r="B98" s="3">
+        <v>46747980</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>197</v>
+        <v>100</v>
+      </c>
+      <c r="B99" s="3">
+        <v>36254168</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>199</v>
+        <v>101</v>
+      </c>
+      <c r="B100" s="3">
+        <v>138359260</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>201</v>
+        <v>102</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1046097350</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102" s="3">
+        <v>89367520</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" s="3">
+        <v>35306730</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" s="3">
+        <v>161916320</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="3">
+        <v>56630220</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1685020160</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="3">
+        <v>77858140</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="3">
+        <v>16080690</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" s="3">
+        <v>147845560</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" s="3">
+        <v>26905500</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" s="3">
+        <v>23352790</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" s="3">
+        <v>23440540</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113" s="3">
+        <v>57736570</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B114" s="3">
+        <v>49414030</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B115" s="3">
+        <v>40962320</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B116" s="3">
+        <v>66864300</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B117" s="3">
+        <v>182664850</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B118" s="3">
+        <v>56814490</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="3">
+        <v>76725720</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" s="3">
+        <v>417898370</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" s="3">
+        <v>1557513490</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122" s="3">
+        <v>7059380</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" s="3">
+        <v>22469820</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B124" s="3">
+        <v>20514960</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B125" s="3">
+        <v>22080400</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B126" s="3">
+        <v>78609420</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B127" s="3">
+        <v>32228300</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B128" s="3">
+        <v>114041969</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B129" s="3">
+        <v>63025130</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B130" s="3">
+        <v>315304450</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" s="3">
+        <v>49055160</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B132" s="3">
+        <v>439698158</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B133" s="3">
+        <v>1871022910</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B134" s="3">
+        <v>113525020</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B135" s="3">
+        <v>4482100</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B136" s="3">
+        <v>21814830</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" s="3">
+        <v>27271240</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" s="3">
+        <v>175156530</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B139" s="3">
+        <v>58802160</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B140" s="3">
+        <v>108531100</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="3">
+        <v>188852700</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="3">
+        <v>39054530</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" s="3">
+        <v>153977190</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" s="3">
+        <v>285588300</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" s="3">
+        <v>61581620</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="3">
+        <v>129840180</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" s="3">
+        <v>143455650</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" s="3">
+        <v>70748630</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" s="3">
+        <v>1790984691</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9"/>
 </worksheet>

</xml_diff>